<commit_message>
Updates ICEG-Person.eap after last WG
</commit_message>
<xml_diff>
--- a/resources/doc/iceg-person.xlsx
+++ b/resources/doc/iceg-person.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\04-professional\vlaanderen-connect\belgif\person\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\vlaanderen-connect\belgif\ICEGthema-person\resources\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51D65195-7364-455C-88D4-D3BEF82E552A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{366200BC-2805-4708-B626-272C26C6534E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4890" yWindow="-21720" windowWidth="38640" windowHeight="21120" xr2:uid="{0406915F-3C02-46B8-8463-A0714B35B479}"/>
+    <workbookView xWindow="-4995" yWindow="-21720" windowWidth="38640" windowHeight="21120" xr2:uid="{0406915F-3C02-46B8-8463-A0714B35B479}"/>
   </bookViews>
   <sheets>
     <sheet name="legal-its" sheetId="4" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="328">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="333">
   <si>
     <t>ENG</t>
   </si>
@@ -1080,9 +1080,6 @@
     <t>citizenship</t>
   </si>
   <si>
-    <t>household</t>
-  </si>
-  <si>
     <t>contact</t>
   </si>
   <si>
@@ -1117,6 +1114,24 @@
   </si>
   <si>
     <t>decision</t>
+  </si>
+  <si>
+    <t>personrelation</t>
+  </si>
+  <si>
+    <t>Generic Identifier</t>
+  </si>
+  <si>
+    <t>Codelist</t>
+  </si>
+  <si>
+    <t>Alias / Pseudoniem?</t>
+  </si>
+  <si>
+    <t>In principle no multivalued allowed</t>
+  </si>
+  <si>
+    <t>Explain TemporalPosition and time modeling.</t>
   </si>
 </sst>
 </file>
@@ -1555,22 +1570,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32297621-32F1-44DF-8D01-BCC564F982D1}">
-  <dimension ref="A1:H54"/>
+  <dimension ref="A1:H53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="21.88671875" style="14" customWidth="1"/>
     <col min="2" max="2" width="8.88671875" style="10"/>
-    <col min="3" max="3" width="88.88671875" style="11" customWidth="1"/>
+    <col min="3" max="3" width="61.109375" style="11" customWidth="1"/>
     <col min="4" max="4" width="8.88671875" style="11"/>
     <col min="5" max="5" width="25.109375" style="11" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="77.33203125" style="10" customWidth="1"/>
-    <col min="7" max="7" width="143.77734375" style="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.88671875" style="11"/>
+    <col min="7" max="7" width="88.44140625" style="10" customWidth="1"/>
+    <col min="8" max="8" width="35.33203125" style="11" customWidth="1"/>
+    <col min="9" max="16384" width="8.88671875" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.3">
@@ -1596,12 +1612,12 @@
         <v>5</v>
       </c>
       <c r="H1" s="15" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>9</v>
@@ -1621,10 +1637,13 @@
       <c r="G2" s="12" t="s">
         <v>269</v>
       </c>
+      <c r="H2" s="11" t="s">
+        <v>328</v>
+      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>14</v>
@@ -1638,10 +1657,13 @@
       <c r="E3" s="11" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="H3" s="11" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="62.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>26</v>
@@ -1661,10 +1683,13 @@
       <c r="G4" s="12" t="s">
         <v>277</v>
       </c>
+      <c r="H4" s="11" t="s">
+        <v>330</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B5" s="10" t="s">
         <v>30</v>
@@ -1681,10 +1706,13 @@
       <c r="F5" s="10" t="s">
         <v>278</v>
       </c>
+      <c r="H5" s="11" t="s">
+        <v>331</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>34</v>
@@ -1744,6 +1772,9 @@
       <c r="F8" s="10" t="s">
         <v>296</v>
       </c>
+      <c r="H8" s="11" t="s">
+        <v>332</v>
+      </c>
     </row>
     <row r="9" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="14" t="s">
@@ -2163,7 +2194,7 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="14" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B28" s="10" t="s">
         <v>145</v>
@@ -2183,7 +2214,7 @@
     </row>
     <row r="29" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A29" s="14" t="s">
-        <v>315</v>
+        <v>327</v>
       </c>
       <c r="B29" s="10" t="s">
         <v>70</v>
@@ -2206,7 +2237,7 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="14" t="s">
-        <v>315</v>
+        <v>327</v>
       </c>
       <c r="B30" s="10" t="s">
         <v>167</v>
@@ -2223,7 +2254,7 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="14" t="s">
-        <v>315</v>
+        <v>327</v>
       </c>
       <c r="B31" s="10" t="s">
         <v>163</v>
@@ -2240,7 +2271,7 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="14" t="s">
-        <v>315</v>
+        <v>327</v>
       </c>
       <c r="B32" s="10" t="s">
         <v>162</v>
@@ -2263,7 +2294,7 @@
     </row>
     <row r="33" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A33" s="14" t="s">
-        <v>315</v>
+        <v>327</v>
       </c>
       <c r="B33" s="10" t="s">
         <v>169</v>
@@ -2283,7 +2314,7 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="14" t="s">
-        <v>315</v>
+        <v>327</v>
       </c>
       <c r="B34" s="10" t="s">
         <v>170</v>
@@ -2298,92 +2329,115 @@
         <v>151</v>
       </c>
     </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35" s="14" t="s">
+        <v>321</v>
+      </c>
+      <c r="B35" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C35" s="11" t="s">
+        <v>216</v>
+      </c>
+      <c r="D35" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E35" s="11" t="s">
+        <v>270</v>
+      </c>
+      <c r="G35" s="10" t="s">
+        <v>291</v>
+      </c>
+    </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="C36" s="11" t="s">
         <v>322</v>
       </c>
-      <c r="B36" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="C36" s="11" t="s">
-        <v>216</v>
-      </c>
-      <c r="D36" s="11" t="s">
-        <v>27</v>
-      </c>
       <c r="E36" s="11" t="s">
-        <v>270</v>
-      </c>
-      <c r="G36" s="10" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+        <v>200</v>
+      </c>
+      <c r="F36" s="10" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A37" s="14" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="C37" s="11" t="s">
-        <v>323</v>
+        <v>221</v>
+      </c>
+      <c r="D37" s="11" t="s">
+        <v>10</v>
       </c>
       <c r="E37" s="11" t="s">
-        <v>200</v>
-      </c>
-      <c r="F37" s="10" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+        <v>151</v>
+      </c>
+      <c r="F37" s="12" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="14" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>188</v>
+        <v>123</v>
       </c>
       <c r="C38" s="11" t="s">
-        <v>221</v>
+        <v>97</v>
       </c>
       <c r="D38" s="11" t="s">
         <v>10</v>
       </c>
       <c r="E38" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="F38" s="12" t="s">
-        <v>298</v>
+        <v>270</v>
+      </c>
+      <c r="G38" s="10" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="14" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B39" s="10" t="s">
-        <v>123</v>
+        <v>186</v>
       </c>
       <c r="C39" s="11" t="s">
-        <v>97</v>
+        <v>234</v>
       </c>
       <c r="D39" s="11" t="s">
         <v>10</v>
       </c>
       <c r="E39" s="11" t="s">
-        <v>270</v>
+        <v>274</v>
+      </c>
+      <c r="F39" s="10" t="s">
+        <v>272</v>
       </c>
       <c r="G39" s="10" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="14" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C40" s="11" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="D40" s="11" t="s">
         <v>10</v>
@@ -2395,67 +2449,67 @@
         <v>272</v>
       </c>
       <c r="G40" s="10" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A41" s="14" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B41" s="10" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="C41" s="11" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="D41" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E41" s="11" t="s">
+        <v>270</v>
+      </c>
+      <c r="F41" s="12" t="s">
+        <v>272</v>
+      </c>
+      <c r="G41" s="12" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A42" s="14" t="s">
+        <v>318</v>
+      </c>
+      <c r="B42" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="C42" s="11" t="s">
+        <v>237</v>
+      </c>
+      <c r="D42" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="E41" s="11" t="s">
+      <c r="E42" s="11" t="s">
         <v>274</v>
       </c>
-      <c r="F41" s="10" t="s">
+      <c r="F42" s="10" t="s">
         <v>272</v>
       </c>
-      <c r="G41" s="10" t="s">
+      <c r="G42" s="10" t="s">
         <v>303</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A42" s="14" t="s">
-        <v>319</v>
-      </c>
-      <c r="B42" s="10" t="s">
-        <v>193</v>
-      </c>
-      <c r="C42" s="11" t="s">
-        <v>236</v>
-      </c>
-      <c r="D42" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="E42" s="11" t="s">
-        <v>270</v>
-      </c>
-      <c r="F42" s="12" t="s">
-        <v>272</v>
-      </c>
-      <c r="G42" s="12" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="14" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B43" s="10" t="s">
-        <v>196</v>
+        <v>244</v>
       </c>
       <c r="C43" s="11" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="D43" s="11" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="E43" s="11" t="s">
         <v>274</v>
@@ -2464,21 +2518,21 @@
         <v>272</v>
       </c>
       <c r="G43" s="10" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="14" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C44" s="11" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="D44" s="11" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="E44" s="11" t="s">
         <v>274</v>
@@ -2487,21 +2541,21 @@
         <v>272</v>
       </c>
       <c r="G44" s="10" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="14" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B45" s="10" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C45" s="11" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="D45" s="11" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="E45" s="11" t="s">
         <v>274</v>
@@ -2513,38 +2567,35 @@
         <v>303</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A46" s="14" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="C46" s="11" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="D46" s="11" t="s">
         <v>27</v>
       </c>
       <c r="E46" s="11" t="s">
-        <v>274</v>
-      </c>
-      <c r="F46" s="10" t="s">
-        <v>272</v>
-      </c>
-      <c r="G46" s="10" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+        <v>270</v>
+      </c>
+      <c r="G46" s="12" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" s="14" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B47" s="10" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="C47" s="11" t="s">
-        <v>241</v>
+        <v>110</v>
       </c>
       <c r="D47" s="11" t="s">
         <v>27</v>
@@ -2552,39 +2603,42 @@
       <c r="E47" s="11" t="s">
         <v>270</v>
       </c>
-      <c r="G47" s="12" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G47" s="10" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A48" s="14" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B48" s="10" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="C48" s="11" t="s">
-        <v>110</v>
+        <v>243</v>
       </c>
       <c r="D48" s="11" t="s">
         <v>27</v>
       </c>
       <c r="E48" s="11" t="s">
-        <v>270</v>
+        <v>151</v>
+      </c>
+      <c r="F48" s="12" t="s">
+        <v>279</v>
       </c>
       <c r="G48" s="10" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" s="14" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B49" s="10" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="C49" s="11" t="s">
-        <v>243</v>
+        <v>250</v>
       </c>
       <c r="D49" s="11" t="s">
         <v>27</v>
@@ -2592,22 +2646,19 @@
       <c r="E49" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="F49" s="12" t="s">
-        <v>279</v>
-      </c>
-      <c r="G49" s="10" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F49" s="10" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A50" s="14" t="s">
         <v>319</v>
       </c>
       <c r="B50" s="10" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="C50" s="11" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="D50" s="11" t="s">
         <v>27</v>
@@ -2615,90 +2666,70 @@
       <c r="E50" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="F50" s="10" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F50" s="12" t="s">
+        <v>279</v>
+      </c>
+      <c r="G50" s="10" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" s="14" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="B51" s="10" t="s">
-        <v>255</v>
+        <v>50</v>
       </c>
       <c r="C51" s="11" t="s">
-        <v>252</v>
+        <v>242</v>
       </c>
       <c r="D51" s="11" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="E51" s="11" t="s">
+        <v>270</v>
+      </c>
+      <c r="G51" s="12" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A52" s="14" t="s">
+        <v>316</v>
+      </c>
+      <c r="B52" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C52" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="D52" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E52" s="11" t="s">
+        <v>274</v>
+      </c>
+      <c r="F52" s="12" t="s">
+        <v>273</v>
+      </c>
+      <c r="G52" s="12" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B53" s="10" t="s">
+        <v>225</v>
+      </c>
+      <c r="C53" s="13" t="s">
+        <v>218</v>
+      </c>
+      <c r="D53" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E53" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="F51" s="12" t="s">
-        <v>279</v>
-      </c>
-      <c r="G51" s="10" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A52" s="14" t="s">
-        <v>317</v>
-      </c>
-      <c r="B52" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="C52" s="11" t="s">
-        <v>242</v>
-      </c>
-      <c r="D52" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="E52" s="11" t="s">
-        <v>270</v>
-      </c>
-      <c r="G52" s="12" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A53" s="14" t="s">
-        <v>317</v>
-      </c>
-      <c r="B53" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="C53" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="D53" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="E53" s="11" t="s">
-        <v>274</v>
-      </c>
-      <c r="F53" s="12" t="s">
-        <v>273</v>
-      </c>
-      <c r="G53" s="12" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B54" s="10" t="s">
-        <v>225</v>
-      </c>
-      <c r="C54" s="13" t="s">
-        <v>218</v>
-      </c>
-      <c r="D54" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="E54" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="G54" s="10" t="s">
+      <c r="G53" s="10" t="s">
         <v>294</v>
       </c>
     </row>
@@ -2726,9 +2757,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:K63"/>
   <sheetViews>
-    <sheetView topLeftCell="A47" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A30" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G59" sqref="G59"/>
+      <selection pane="topRight" activeCell="A61" sqref="A61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -2747,7 +2778,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>0</v>
@@ -3846,7 +3877,7 @@
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
   </sheetData>
@@ -3855,6 +3886,35 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_x0063_bw3 xmlns="d8af5a5f-e2e6-468c-9f28-f81d99523fed">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </_x0063_bw3>
+    <y2ot xmlns="d8af5a5f-e2e6-468c-9f28-f81d99523fed" xsi:nil="true"/>
+    <Comment xmlns="d8af5a5f-e2e6-468c-9f28-f81d99523fed" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="d8af5a5f-e2e6-468c-9f28-f81d99523fed">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="9a9ec0f0-7796-43d0-ac1f-4c8c46ee0bd1" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007D2FA61B056BF04BB41EAF8746BED8CA" ma:contentTypeVersion="23" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1130e86534d713d523efcecbbffa1ece">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="abd5de4e-6ecd-4522-a9f4-1c24c7648312" xmlns:ns3="d8af5a5f-e2e6-468c-9f28-f81d99523fed" xmlns:ns4="9a9ec0f0-7796-43d0-ac1f-4c8c46ee0bd1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="42270d1cb4c674c32b17caee095c08f5" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="abd5de4e-6ecd-4522-a9f4-1c24c7648312"/>
@@ -4148,36 +4208,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_x0063_bw3 xmlns="d8af5a5f-e2e6-468c-9f28-f81d99523fed">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </_x0063_bw3>
-    <y2ot xmlns="d8af5a5f-e2e6-468c-9f28-f81d99523fed" xsi:nil="true"/>
-    <Comment xmlns="d8af5a5f-e2e6-468c-9f28-f81d99523fed" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="d8af5a5f-e2e6-468c-9f28-f81d99523fed">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="9a9ec0f0-7796-43d0-ac1f-4c8c46ee0bd1" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9FE5619E-A92B-4C98-9460-A917041C2909}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C2845976-DF44-46D2-8288-F30B8F4D993A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="d8af5a5f-e2e6-468c-9f28-f81d99523fed"/>
+    <ds:schemaRef ds:uri="9a9ec0f0-7796-43d0-ac1f-4c8c46ee0bd1"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{92CB412D-DD23-4721-88BB-F07F6E6F7239}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4195,23 +4245,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C2845976-DF44-46D2-8288-F30B8F4D993A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="d8af5a5f-e2e6-468c-9f28-f81d99523fed"/>
-    <ds:schemaRef ds:uri="9a9ec0f0-7796-43d0-ac1f-4c8c46ee0bd1"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9FE5619E-A92B-4C98-9460-A917041C2909}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>